<commit_message>
Log file feature added, query for distance calculation changed.
</commit_message>
<xml_diff>
--- a/LBS_10_ExcelBasedLBS/pois.xlsx
+++ b/LBS_10_ExcelBasedLBS/pois.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="20" windowWidth="38400" windowHeight="22340" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
   <si>
     <t>Inside AR</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Metaio Office</t>
   </si>
   <si>
-    <t>Metaio is a n Augmented Reality (AR) company that develops software technology and provides augmented reality solutions</t>
-  </si>
-  <si>
     <t>49-(0)89-5480-198-0</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Oktoberfest</t>
   </si>
   <si>
-    <t>Oktoberfest is the worlds largest funfair held annually in Munich, Bavaria, Germany</t>
-  </si>
-  <si>
     <t>49 (0)89 233 965 00</t>
   </si>
   <si>
@@ -159,15 +153,6 @@
     <t>Capital of United Arab Emirates</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Flag_of_the_United_Arab_Emirates.svg/188px-Flag_of_the_United_Arab_Emirates.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/c/cd/United_Arab_Emirates_%28orthographic_projection%29.svg/500px-United_Arab_Emirates_%28orthographic_projection%29.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Flag_of_the_United_Arab_Emirates.svg/125px-Flag_of_the_United_Arab_Emirates.svg.png</t>
-  </si>
-  <si>
     <t>http://government.ae/en</t>
   </si>
   <si>
@@ -177,15 +162,6 @@
     <t>Capital of Germany</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/b/ba/Flag_of_Germany.svg/125px-Flag_of_Germany.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/b/ba/Flag_of_Germany.svg/250px-Flag_of_Germany.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/2/26/EU-Germany.svg/250px-EU-Germany.svg.png</t>
-  </si>
-  <si>
     <t>http://en.wikipedia.org/wiki/Germany</t>
   </si>
   <si>
@@ -198,15 +174,6 @@
     <t>http://en.wikipedia.org/wiki/Australia</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/8/88/Flag_of_Australia_%28converted%29.svg/125px-Flag_of_Australia_%28converted%29.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/8/88/Flag_of_Australia_%28converted%29.svg/188px-Flag_of_Australia_%28converted%29.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28ortho…ic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png</t>
-  </si>
-  <si>
     <t>Doha</t>
   </si>
   <si>
@@ -216,15 +183,6 @@
     <t>http://en.wikipedia.org/wiki/Qatar</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/6/65/Flag_of_Qatar.svg/125px-Flag_of_Qatar.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/6/65/Flag_of_Qatar.svg/188px-Flag_of_Qatar.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/d/d4/QAT_orthographic.svg/375px-QAT_orthographic.svg.png</t>
-  </si>
-  <si>
     <t>48.142516</t>
   </si>
   <si>
@@ -282,15 +240,6 @@
     <t>http://en.wikipedia.org/wiki/Pakistan</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/3/32/Flag_of_Pakistan.svg/125px-Flag_of_Pakistan.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/3/32/Flag_of_Pakistan.svg/188px-Flag_of_Pakistan.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/b/b6/Pakistan_%28orthographic_projection%29.svg/330px-Pakistan_%28orthographic_projection%29.svg.png</t>
-  </si>
-  <si>
     <t>33.7167</t>
   </si>
   <si>
@@ -306,15 +255,6 @@
     <t>http://en.wikipedia.org/wiki/United_Kingdom</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/a/ae/Flag_of_the_United_Kingdom.svg/125px-Flag_of_the_United_Kingdom.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/a/ae/Flag_of_the_United_Kingdom.svg/188px-Flag_of_the_United_Kingdom.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/d/d1/EU-United_Kingdom.svg/250px-EU-United_Kingdom.svg.png</t>
-  </si>
-  <si>
     <t>51.5072</t>
   </si>
   <si>
@@ -330,15 +270,6 @@
     <t>http://en.wikipedia.org/wiki/Norway</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/d/d9/Flag_of_Norway.svg/125px-Flag_of_Norway.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/d/d9/Flag_of_Norway.svg/188px-Flag_of_Norway.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/0/01/Europe-Norway.svg/375px-Europe-Norway.svg.png</t>
-  </si>
-  <si>
     <t>59.9500</t>
   </si>
   <si>
@@ -354,12 +285,6 @@
     <t>http://en.wikipedia.org/wiki/Sweden</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/4/4c/Flag_of_Sweden.svg/188px-Flag_of_Sweden.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/0/06/EU-Sweden.svg/375px-EU-Sweden.svg.png</t>
-  </si>
-  <si>
     <t>59.3294</t>
   </si>
   <si>
@@ -375,19 +300,43 @@
     <t>http://en.wikipedia.org/wiki/United_States</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/a/a4/Flag_of_the_United_States.svg/125px-Flag_of_the_United_States.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/en/thumb/a/a4/Flag_of_the_United_States.svg/188px-Flag_of_the_United_States.svg.png</t>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/d/dc/USA_orthographic.svg/330px-USA_orthographic.svg.png</t>
-  </si>
-  <si>
     <t>47.5000</t>
   </si>
   <si>
     <t>120.5000</t>
+  </si>
+  <si>
+    <t>resources/UAE.png</t>
+  </si>
+  <si>
+    <t>resources/Germany.png</t>
+  </si>
+  <si>
+    <t>resources/Australia.png</t>
+  </si>
+  <si>
+    <t>resources/Qatar.png</t>
+  </si>
+  <si>
+    <t>resources/Pakistan.png</t>
+  </si>
+  <si>
+    <t>resources/UK.png</t>
+  </si>
+  <si>
+    <t>resources/Norway.png</t>
+  </si>
+  <si>
+    <t>resources/Sweden.png</t>
+  </si>
+  <si>
+    <t>resources/US.png</t>
+  </si>
+  <si>
+    <t>Metaio is an Augmented Reality (AR) company that develops software technology and provides augmented reality solutions</t>
+  </si>
+  <si>
+    <t>Oktoberfest is the worlds largest funfair held annually in Munich, Bavaria, Germany</t>
   </si>
 </sst>
 </file>
@@ -785,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -874,13 +823,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="75">
@@ -891,34 +840,34 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45">
@@ -926,37 +875,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="60">
@@ -964,197 +913,197 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="60">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="M8" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="N9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="N10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="49">
@@ -1162,97 +1111,97 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>95</v>
+        <v>76</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="I11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="N13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="45">
@@ -1260,57 +1209,53 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>118</v>
+        <v>92</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="N14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2" tooltip="Abu Dhabi"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Flag_of_the_United_Arab_Emirates.svg/125px-Flag_of_the_United_Arab_Emirates.svg.png"/>
+    <hyperlink ref="G6" r:id="rId3" display="http://upload.wikimedia.org/wikipedia/commons/thumb/c/cd/United_Arab_Emirates_%28orthographic_projection%29.svg/500px-United_Arab_Emirates_%28orthographic_projection%29.svg.png"/>
+    <hyperlink ref="F6" r:id="rId4" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Flag_of_the_United_Arab_Emirates.svg/125px-Flag_of_the_United_Arab_Emirates.svg.png" display="http://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Flag_of_the_United_Arab_Emirates.svg/125px-Flag_of_the_United_Arab_Emirates.svg.png"/>
     <hyperlink ref="B7" r:id="rId5" tooltip="Berlin"/>
-    <hyperlink ref="F7" r:id="rId6" tooltip="http://upload.wikimedia.org/wikipedia/en/thumb/b/ba/Flag_of_Germany.svg/125px-Flag_of_Germany.svg.png"/>
-    <hyperlink ref="H7" r:id="rId7" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/2/26/EU-Germany.svg/250px-EU-Germany.svg.png"/>
+    <hyperlink ref="F7" r:id="rId6" tooltip="http://upload.wikimedia.org/wikipedia/en/thumb/b/ba/Flag_of_Germany.svg/125px-Flag_of_Germany.svg.png" display="http://upload.wikimedia.org/wikipedia/en/thumb/b/ba/Flag_of_Germany.svg/125px-Flag_of_Germany.svg.png"/>
+    <hyperlink ref="H7" r:id="rId7" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/2/26/EU-Germany.svg/250px-EU-Germany.svg.png" display="http://upload.wikimedia.org/wikipedia/commons/thumb/2/26/EU-Germany.svg/250px-EU-Germany.svg.png"/>
     <hyperlink ref="B8" r:id="rId8" tooltip="Canberra"/>
-    <hyperlink ref="F8" r:id="rId9" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/8/88/Flag_of_Australia_%28converted%29.svg/125px-Flag_of_Australia_%28converted%29.svg.png"/>
-    <hyperlink ref="H8" r:id="rId10" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28orthographic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png"/>
-    <hyperlink ref="B9" r:id="rId11" tooltip="Doha"/>
-    <hyperlink ref="F9" r:id="rId12" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/6/65/Flag_of_Qatar.svg/125px-Flag_of_Qatar.svg.png"/>
-    <hyperlink ref="B10" r:id="rId13" tooltip="Islamabad"/>
-    <hyperlink ref="F10" r:id="rId14" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/3/32/Flag_of_Pakistan.svg/125px-Flag_of_Pakistan.svg.png"/>
-    <hyperlink ref="B11" r:id="rId15" tooltip="London"/>
-    <hyperlink ref="F11" r:id="rId16" tooltip="http://upload.wikimedia.org/wikipedia/en/thumb/a/ae/Flag_of_the_United_Kingdom.svg/125px-Flag_of_the_United_Kingdom.svg.png"/>
-    <hyperlink ref="H11" r:id="rId17" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/d/d1/EU-United_Kingdom.svg/250px-EU-United_Kingdom.svg.png"/>
-    <hyperlink ref="B12" r:id="rId18" tooltip="Oslo"/>
-    <hyperlink ref="F12" r:id="rId19" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/d/d9/Flag_of_Norway.svg/125px-Flag_of_Norway.svg.png"/>
-    <hyperlink ref="B13" r:id="rId20" tooltip="Stockholm"/>
-    <hyperlink ref="B14" r:id="rId21" tooltip="Washington, D.C."/>
-    <hyperlink ref="F14" r:id="rId22" tooltip="http://upload.wikimedia.org/wikipedia/en/thumb/a/a4/Flag_of_the_United_States.svg/125px-Flag_of_the_United_States.svg.png"/>
+    <hyperlink ref="H8" r:id="rId9" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28orthographic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png" display="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28ortho…ic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png"/>
+    <hyperlink ref="B9" r:id="rId10" tooltip="Doha"/>
+    <hyperlink ref="B10" r:id="rId11" tooltip="Islamabad"/>
+    <hyperlink ref="B11" r:id="rId12" tooltip="London"/>
+    <hyperlink ref="B12" r:id="rId13" tooltip="Oslo"/>
+    <hyperlink ref="B13" r:id="rId14" tooltip="Stockholm"/>
+    <hyperlink ref="B14" r:id="rId15" tooltip="Washington, D.C."/>
+    <hyperlink ref="G8" r:id="rId16" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28orthographic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png" display="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28ortho…ic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png"/>
+    <hyperlink ref="F8" r:id="rId17" tooltip="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28orthographic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png" display="http://upload.wikimedia.org/wikipedia/commons/thumb/7/7d/Australia_%28ortho…ic_projection%29.svg/220px-Australia_%28orthographic_projection%29.svg.png"/>
+    <hyperlink ref="E11" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>